<commit_message>
list user + status
</commit_message>
<xml_diff>
--- a/WebContent/WEB-INF/template/excel/report_index_data_daily.xlsx
+++ b/WebContent/WEB-INF/template/excel/report_index_data_daily.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Toa hang ngay" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Bao cao mat hang" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">BÁO CÁO TIẾN ĐỘ GỬI TOA HÀNG NGÀY</t>
   </si>
@@ -73,16 +73,39 @@
   </si>
   <si>
     <t xml:space="preserve">Số ngày gửi trể</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THỐNG KÊ SỐ THÙNG HÀNG THEO TOA NHẬP HẰNG NGÀY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày thống kê:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày nhận:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mặt hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên Cấp 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng số thùng đã nhận trong niên vụ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Số thùng phát sinh trong ngày nhận</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -113,6 +136,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -122,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -137,6 +168,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -163,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,6 +228,26 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -211,7 +269,7 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -219,17 +277,17 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.67611336032389"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -247,6 +305,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
+      <c r="M1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
@@ -260,6 +319,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
+      <c r="M2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -279,6 +339,7 @@
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
+      <c r="M3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
@@ -292,6 +353,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
+      <c r="M4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -360,17 +422,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="51.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>